<commit_message>
Added description of input data files
Added detailed description of input data files.
Improved documentation of parameters in parameter input file (including examples of how to fill in reach structure parameters)
</commit_message>
<xml_diff>
--- a/Development/v0-2/Parameters_working.xlsx
+++ b/Development/v0-2/Parameters_working.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="259">
   <si>
     <t>Param</t>
   </si>
@@ -201,9 +201,6 @@
     <t>kg/m2</t>
   </si>
   <si>
-    <t>Soil mass per m2</t>
-  </si>
-  <si>
     <t>Soil depth</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>Net annual P input to the soil (may be negative if have more uptake than input)</t>
   </si>
   <si>
-    <t>A value only needs to be supplied when the model is run in validation mode. In calibration mode, it is calculated within the model and output as Kf</t>
-  </si>
-  <si>
     <t>S_Ar</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
   </si>
   <si>
     <t>Reach slope (ideally length-weighted)</t>
-  </si>
-  <si>
-    <t>Vegetation cover factor, describing ratio between long-term erosion under the land use class, compared to under bare soil of the same soil type, slope, etc. Sourced from (R)USLE literature.</t>
   </si>
   <si>
     <t>C_cover</t>
@@ -672,9 +663,6 @@
     <t>Only for A and S</t>
   </si>
   <si>
-    <t>NC parameter value assigned according to type (defined in 'Constant' sheet)</t>
-  </si>
-  <si>
     <t>Format for value cell</t>
   </si>
   <si>
@@ -696,9 +684,6 @@
     <t>Simulation start date. If calculating PET, must be near 1st January of given year</t>
   </si>
   <si>
-    <t>Set to 1 unless PET thought to be systematically under or over-estimated by Thornthwaite in the study area</t>
-  </si>
-  <si>
     <t>C:\Data\SimplyP_Local\Applications\Morsa\met_obs_PT_dateOffset.csv</t>
   </si>
   <si>
@@ -822,10 +807,38 @@
     <t>all</t>
   </si>
   <si>
-    <t>Initial in-stream flow for one sub-catchment. A value &gt;0 is required for one sub-catchment (area-weighting applied to calculate in all other sub-catchments)</t>
-  </si>
-  <si>
     <t>Calibrated to give appropriate long-term response. Only needed if simulating dynamic soil water TDP and labile soil P</t>
+  </si>
+  <si>
+    <t>Area-weighted over different land use classes and soils present in the catchment</t>
+  </si>
+  <si>
+    <t>Set to 1 unless PET thought to be systematically under or over-estimated by Thornthwaite in the study area. If necessary, area-weight over the different land cover classes present</t>
+  </si>
+  <si>
+    <t>Initial in-stream flow for one sub-catchment</t>
+  </si>
+  <si>
+    <t>A value &gt;0 is required for one sub-catchment</t>
+  </si>
+  <si>
+    <t>Soil mass per m2 on agricultural land</t>
+  </si>
+  <si>
+    <t>A value only needs to be supplied when the model is run in validation mode. In calibration mode, it is calculated within the model and output as Kf (see the print statement after running the model)</t>
+  </si>
+  <si>
+    <t>NC parameter value is assigned within the model according to the type of newly-converted land</t>
+  </si>
+  <si>
+    <t>Combined vegetation cover and soil erodibility factor. The vegetation cover factor describes the ratio between long-term erosion under the land class, compared to under bare soil of the same soil type, slope, etc. This factor can also include differences in inherent soil erodibility between different land use classes (e.g. due to texture and organic matter content)</t>
+  </si>
+  <si>
+    <t>NC parameter value is assigned within the model according to the type of newly-converted land
+Values can be sourced from (R)USLE literature. Differences in inherent soil erodibility are generally termed the K factor in USLE-related literature.</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1664,6 +1677,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1904,6 +1920,118 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5063490" y="0"/>
+          <a:ext cx="6503670" cy="4457700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Examples:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>118576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>184810</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="51023"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5372099" y="118576"/>
+          <a:ext cx="5431181" cy="3958124"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2271,356 +2399,356 @@
         <v>24</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C10" s="32">
         <v>3</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="38" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="38" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="40" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="43" t="s">
         <v>140</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C21" s="32">
         <v>300</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="38" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="38" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B25" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="43" t="s">
         <v>152</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" s="43" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D26" s="45" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2631,10 +2759,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2646,13 +2774,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2670,8 +2798,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2680,7 +2814,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2696,7 +2830,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="97" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="94" t="s">
         <v>0</v>
@@ -2717,18 +2851,18 @@
         <v>3</v>
       </c>
       <c r="H1" s="96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="103" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="98" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="99" t="s">
         <v>11</v>
@@ -2745,12 +2879,12 @@
       <c r="G2" s="101"/>
       <c r="H2" s="102"/>
       <c r="I2" s="131" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="109" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="104" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B3" s="105" t="s">
         <v>6</v>
@@ -2759,7 +2893,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="106" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E3" s="163">
         <v>1200</v>
@@ -2770,12 +2904,12 @@
       <c r="G3" s="107"/>
       <c r="H3" s="108"/>
       <c r="I3" s="132" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="109" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="110" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" s="111" t="s">
         <v>7</v>
@@ -2784,7 +2918,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="112" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="150">
         <v>10</v>
@@ -2797,12 +2931,12 @@
         <v>-5</v>
       </c>
       <c r="I4" s="133" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="116" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B5" s="117" t="s">
         <v>8</v>
@@ -2811,7 +2945,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="118" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E5" s="176">
         <v>0.3</v>
@@ -2822,21 +2956,21 @@
       <c r="G5" s="120"/>
       <c r="H5" s="121"/>
       <c r="I5" s="134" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="126" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="126" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="122" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C6" s="123" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="124" t="s">
-        <v>96</v>
+        <v>256</v>
       </c>
       <c r="E6" s="172">
         <v>0.5</v>
@@ -2849,21 +2983,21 @@
       </c>
       <c r="H6" s="125"/>
       <c r="I6" s="135" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="126" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="128" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="128" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="129" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E7" s="152">
         <v>0</v>
@@ -2876,7 +3010,7 @@
       </c>
       <c r="H7" s="130"/>
       <c r="I7" s="136" t="s">
-        <v>203</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +3036,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -2925,7 +3059,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>18</v>
@@ -2951,7 +3085,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>20</v>
@@ -2960,7 +3094,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E3" s="27">
         <v>1</v>
@@ -2977,7 +3111,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>19</v>
@@ -2986,7 +3120,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E4" s="27">
         <v>0</v>
@@ -3003,7 +3137,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>21</v>
@@ -3012,7 +3146,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E5" s="27">
         <v>0</v>
@@ -3029,16 +3163,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="27">
         <v>0</v>
@@ -3055,16 +3189,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="27">
         <v>0</v>
@@ -3081,16 +3215,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="27">
         <v>0</v>
@@ -3107,16 +3241,16 @@
     </row>
     <row r="9" spans="1:9" s="181" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="183" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C9" s="183" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="183" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E9" s="185">
         <v>0.65</v>
@@ -3133,16 +3267,16 @@
     </row>
     <row r="10" spans="1:9" s="181" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="183" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="183" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="183" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E10" s="184">
         <v>4</v>
@@ -3159,16 +3293,16 @@
     </row>
     <row r="11" spans="1:9" s="181" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="183" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" s="183" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="183" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" s="184">
         <v>4</v>
@@ -3185,16 +3319,16 @@
     </row>
     <row r="12" spans="1:9" s="181" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" s="183" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="183" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E12" s="184">
         <v>10</v>
@@ -3211,7 +3345,7 @@
     </row>
     <row r="13" spans="1:9" s="187" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="186" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="187" t="s">
         <v>22</v>
@@ -3237,7 +3371,7 @@
     </row>
     <row r="14" spans="1:9" s="181" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="178" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="179" t="s">
         <v>23</v>
@@ -3246,7 +3380,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="179" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E14" s="180">
         <v>0.5</v>
@@ -3263,7 +3397,7 @@
     </row>
     <row r="15" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>29</v>
@@ -3284,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="84" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I15" s="160">
         <v>0</v>
@@ -3292,7 +3426,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3305,8 +3439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3322,7 +3456,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -3337,61 +3471,61 @@
         <v>24</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2" s="59" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" s="59">
         <v>50</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="66" t="s">
-        <v>104</v>
-      </c>
       <c r="C3" s="66" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D3" s="66" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E3" s="154">
         <v>2.74</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C4" s="59" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E4" s="59">
         <v>59.596699999999998</v>
@@ -3400,10 +3534,10 @@
     </row>
     <row r="5" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C5" s="63" t="s">
         <v>17</v>
@@ -3415,12 +3549,12 @@
         <v>0.02</v>
       </c>
       <c r="F5" s="64" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="192" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="192" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="189" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="190" t="s">
         <v>5</v>
@@ -3435,12 +3569,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="191" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="61" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="63" t="s">
         <v>4</v>
@@ -3449,16 +3583,18 @@
         <v>12</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E7" s="159">
         <v>200</v>
       </c>
-      <c r="F7" s="64"/>
+      <c r="F7" s="64" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="63" t="s">
         <v>25</v>
@@ -3476,7 +3612,7 @@
     </row>
     <row r="9" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="63" t="s">
         <v>26</v>
@@ -3494,7 +3630,7 @@
     </row>
     <row r="10" spans="1:7" s="61" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="63" t="s">
         <v>27</v>
@@ -3512,10 +3648,10 @@
     </row>
     <row r="11" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C11" s="63" t="s">
         <v>53</v>
@@ -3530,10 +3666,10 @@
     </row>
     <row r="12" spans="1:7" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="87" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="88" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C12" s="88" t="s">
         <v>17</v>
@@ -3545,12 +3681,12 @@
         <v>0.42</v>
       </c>
       <c r="F12" s="90" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="63" t="s">
         <v>28</v>
@@ -3559,38 +3695,40 @@
         <v>56</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E13" s="177">
         <v>0.4</v>
       </c>
-      <c r="F13" s="177"/>
+      <c r="F13" s="208" t="s">
+        <v>252</v>
+      </c>
       <c r="G13" s="177"/>
     </row>
     <row r="14" spans="1:7" s="198" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="193" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="194" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C14" s="194" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="194" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E14" s="195">
         <v>1</v>
       </c>
       <c r="F14" s="196" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G14" s="197"/>
     </row>
     <row r="15" spans="1:7" s="204" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="201" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B15" s="202" t="s">
         <v>32</v>
@@ -3599,38 +3737,38 @@
         <v>57</v>
       </c>
       <c r="D15" s="202" t="s">
-        <v>58</v>
+        <v>253</v>
       </c>
       <c r="E15" s="199">
         <v>95</v>
       </c>
       <c r="F15" s="203" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="204" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="204" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="205" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B16" s="206" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="206" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="206" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E16" s="200">
         <v>1.1315280460000001E-4</v>
       </c>
       <c r="F16" s="207" t="s">
-        <v>84</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="77" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="76" t="s">
         <v>30</v>
@@ -3639,38 +3777,38 @@
         <v>15</v>
       </c>
       <c r="D17" s="76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="173">
         <v>0</v>
       </c>
       <c r="F17" s="168" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="77" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="165" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="166" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C18" s="166" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="166" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E18" s="169">
         <v>0.7</v>
       </c>
       <c r="F18" s="167" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="77" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="79" t="s">
         <v>31</v>
@@ -3679,93 +3817,93 @@
         <v>17</v>
       </c>
       <c r="D19" s="79" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="170">
         <v>1.5</v>
       </c>
       <c r="F19" s="137" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="70" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C20" s="69" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E20" s="171">
         <v>11000</v>
       </c>
       <c r="F20" s="71" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="70" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C21" s="73" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="73" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="174">
         <v>2</v>
       </c>
       <c r="F21" s="74" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="70" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="80" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="81" t="s">
         <v>91</v>
-      </c>
-      <c r="C22" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="81" t="s">
-        <v>93</v>
       </c>
       <c r="E22" s="156">
         <v>60</v>
       </c>
       <c r="F22" s="138" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="70" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="83" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="83" t="s">
         <v>92</v>
-      </c>
-      <c r="C23" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="83" t="s">
-        <v>94</v>
       </c>
       <c r="E23" s="157">
         <v>304</v>
       </c>
       <c r="F23" s="139" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3797,7 +3935,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
@@ -3807,7 +3945,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -3815,7 +3953,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>34</v>
@@ -3835,7 +3973,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -3843,7 +3981,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>35</v>
@@ -3876,32 +4014,32 @@
     </row>
     <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.65">
       <c r="A13" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="54" t="s">
         <v>170</v>
-      </c>
-      <c r="B14" s="54" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>173</v>
       </c>
       <c r="E14" s="55" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
       <c r="A15" s="46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B15" s="47">
         <v>1000</v>
@@ -3913,15 +4051,15 @@
         <v>2650</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
       <c r="A16" s="48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="47">
         <v>10</v>
@@ -3933,15 +4071,15 @@
         <v>30</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="51">
         <f>B15*B16/100</f>
@@ -3962,23 +4100,23 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="42.3" x14ac:dyDescent="0.5">
       <c r="A20" s="147" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B20" s="148" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C20" s="149" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="140" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B21" s="141">
         <v>0.1</v>
@@ -3990,7 +4128,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="140" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B22" s="143">
         <v>1</v>
@@ -4002,7 +4140,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="140" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B23" s="141">
         <v>1.2</v>
@@ -4014,7 +4152,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="140" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B24" s="141">
         <v>1.4</v>
@@ -4026,7 +4164,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="140" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B25" s="141">
         <v>1.35</v>
@@ -4038,7 +4176,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="140" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B26" s="141">
         <v>1.35</v>
@@ -4050,7 +4188,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="140" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B27" s="141">
         <v>1.1000000000000001</v>
@@ -4062,7 +4200,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="140" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B28" s="141">
         <v>1.8</v>
@@ -4074,7 +4212,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="140" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B29" s="141">
         <v>1.7</v>
@@ -4086,7 +4224,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="140" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B30" s="141">
         <v>1.65</v>
@@ -4098,7 +4236,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="144" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B31" s="145">
         <v>2.65</v>

</xml_diff>

<commit_message>
Added description of input and output data files. Minor improvements to v0.2
- Populated the text file with a description of the data formats in the input and output data files.

- Updated model development log text file.

Plus minor improvements to v0.2:

- Improved documentation of functions in model.py

- Add calculation of reach SRP and TP fluxes (previously only concentrations were calculated) and output in reach results dataframes
</commit_message>
<xml_diff>
--- a/Development/v0-2/Parameters_working.xlsx
+++ b/Development/v0-2/Parameters_working.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="258">
   <si>
     <t>Param</t>
   </si>
@@ -836,9 +836,6 @@
   <si>
     <t>NC parameter value is assigned within the model according to the type of newly-converted land
 Values can be sourced from (R)USLE literature. Differences in inherent soil erodibility are generally termed the K factor in USLE-related literature.</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
 </sst>
 </file>
@@ -1929,16 +1926,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>598170</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1947,8 +1944,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5063490" y="0"/>
-          <a:ext cx="6503670" cy="4457700"/>
+          <a:off x="4815840" y="57150"/>
+          <a:ext cx="6503670" cy="6217920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1983,26 +1980,108 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng"/>
+            <a:t>Description</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Column</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> A: Reach number (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>integer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Column</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> B: List of reaches which flow directly into the current reach. Leave blank if none. If more than one, separate reach numbers (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>integers</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>) with a comma. Spacing doesn't matter.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>Column C: Boolean column indicating whether or not the reach should be included in a sum over multiple reaches to calculte total inputs to a receiving waterbody (e.g. a lake or estuary). If not, enter 0 or leave blank. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>If yes, enter 1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>. All rows with '1' entered will be included in the final sum.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" u="sng"/>
+            <a:t>Examples</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Examples:</a:t>
+            <a:t> (the small blue circle at the bottom of the catchment is a lake that we want to calculate total inputs to,</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> as well as calculating results in each sub-catchment separately):</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>118576</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15239</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>169828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>184810</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2024,8 +2103,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5372099" y="118576"/>
-          <a:ext cx="5431181" cy="3958124"/>
+          <a:off x="5513069" y="2181508"/>
+          <a:ext cx="5219701" cy="3804002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2375,7 +2454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2759,10 +2838,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2796,11 +2875,6 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>